<commit_message>
Ejecucion por separado (OK), Corregir bug de carga intermedia entre procesos
</commit_message>
<xml_diff>
--- a/test/input.xlsx
+++ b/test/input.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IMAMANIH\Documents\SeguroVIdaLeyBot\SVL-W3B\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IMAMANIH\Documents\GithubRepos\AQPBOX-SVLBot\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81C916B-0473-4314-9E8B-447D47560BD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214D570B-DB25-4B6E-A738-1959CEF4D943}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9405" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ingresos" sheetId="1" r:id="rId1"/>
+    <sheet name="Ceses" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$598</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingresos!$A$1:$N$598</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6760" uniqueCount="2931">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7002" uniqueCount="2936">
   <si>
     <t>TIPO_DOCUMENTO</t>
   </si>
@@ -8816,16 +8817,33 @@
   </si>
   <si>
     <t>MEIV NEMERIS</t>
+  </si>
+  <si>
+    <t>TIPO DE DOCUMENTO</t>
+  </si>
+  <si>
+    <t>NRO DE DOCUMENTO
+(A 8 DIGITOS)</t>
+  </si>
+  <si>
+    <t>MOTIVO</t>
+  </si>
+  <si>
+    <t>FECHA DE BAJA</t>
+  </si>
+  <si>
+    <t>RENUNCIA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="00000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8839,16 +8857,30 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -8871,16 +8903,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9186,7 +9238,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N598"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="M599" sqref="M599"/>
     </sheetView>
   </sheetViews>
@@ -34269,4 +34321,1706 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3B86A73-E758-4CD1-A3D8-6A9EC4501DA0}">
+  <dimension ref="A1:D120"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="48.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>2931</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2932</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2933</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2934</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>40089227</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D2" s="3">
+        <v>45513</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>2167125</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D3" s="3">
+        <v>45511</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>43131909</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45523</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>41629039</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45530</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>47055452</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D6" s="3">
+        <v>45514</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>44668103</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D7" s="3">
+        <v>45527</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>45219500</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>46590602</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45535</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>42706497</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D10" s="3">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>47073885</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D11" s="3">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>46788506</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D12" s="3">
+        <v>45507</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>43234573</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D13" s="3">
+        <v>45509</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>70188502</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D14" s="3">
+        <v>45519</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>47105689</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D15" s="3">
+        <v>45521</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>46591221</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D16" s="3">
+        <v>45525</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>42318426</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D17" s="3">
+        <v>45524</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>41834611</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D18" s="3">
+        <v>45509</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19">
+        <v>46580868</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D19" s="3">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20">
+        <v>47646875</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D20" s="3">
+        <v>45523</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21">
+        <v>74611301</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D21" s="3">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22">
+        <v>40690076</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D22" s="3">
+        <v>45511</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23">
+        <v>45851361</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D23" s="3">
+        <v>45527</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24">
+        <v>47967780</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D24" s="3">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25">
+        <v>24003265</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D25" s="3">
+        <v>45516</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26">
+        <v>42981463</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D26" s="3">
+        <v>45535</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27">
+        <v>70758414</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D27" s="3">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28">
+        <v>44798732</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D28" s="3">
+        <v>45535</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>46203351</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D29" s="3">
+        <v>45507</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30">
+        <v>46198860</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D30" s="3">
+        <v>45535</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31">
+        <v>76904490</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D31" s="3">
+        <v>45513</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32">
+        <v>43117975</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D32" s="3">
+        <v>45509</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33">
+        <v>44118230</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D33" s="3">
+        <v>45512</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34">
+        <v>47960778</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D34" s="3">
+        <v>45521</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35">
+        <v>47008915</v>
+      </c>
+      <c r="C35" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D35" s="3">
+        <v>45530</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36">
+        <v>45900142</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D36" s="3">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37">
+        <v>70031713</v>
+      </c>
+      <c r="C37" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D37" s="3">
+        <v>45513</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38">
+        <v>72656940</v>
+      </c>
+      <c r="C38" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D38" s="3">
+        <v>45534</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39">
+        <v>73374188</v>
+      </c>
+      <c r="C39" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D39" s="3">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40">
+        <v>72571130</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D40" s="3">
+        <v>45526</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41">
+        <v>72679294</v>
+      </c>
+      <c r="C41" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D41" s="3">
+        <v>45511</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42">
+        <v>47271931</v>
+      </c>
+      <c r="C42" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D42" s="3">
+        <v>45527</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43">
+        <v>42647521</v>
+      </c>
+      <c r="C43" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D43" s="3">
+        <v>45512</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44">
+        <v>70756104</v>
+      </c>
+      <c r="C44" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D44" s="3">
+        <v>45514</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45">
+        <v>70138183</v>
+      </c>
+      <c r="C45" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D45" s="3">
+        <v>45535</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46">
+        <v>71852527</v>
+      </c>
+      <c r="C46" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D46" s="3">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47">
+        <v>44919241</v>
+      </c>
+      <c r="C47" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D47" s="3">
+        <v>45513</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48">
+        <v>74447555</v>
+      </c>
+      <c r="C48" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D48" s="3">
+        <v>45535</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49">
+        <v>70073409</v>
+      </c>
+      <c r="C49" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D49" s="3">
+        <v>45506</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50">
+        <v>73967544</v>
+      </c>
+      <c r="C50" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D50" s="3">
+        <v>45525</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51">
+        <v>76299987</v>
+      </c>
+      <c r="C51" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D51" s="3">
+        <v>45509</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52">
+        <v>41396964</v>
+      </c>
+      <c r="C52" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D52" s="3">
+        <v>45516</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53">
+        <v>43127140</v>
+      </c>
+      <c r="C53" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D53" s="3">
+        <v>45527</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54">
+        <v>70682281</v>
+      </c>
+      <c r="C54" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D54" s="3">
+        <v>45535</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55">
+        <v>44757568</v>
+      </c>
+      <c r="C55" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D55" s="3">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56">
+        <v>46121580</v>
+      </c>
+      <c r="C56" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D56" s="3">
+        <v>45535</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57">
+        <v>46528020</v>
+      </c>
+      <c r="C57" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D57" s="3">
+        <v>45524</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>14</v>
+      </c>
+      <c r="B58">
+        <v>43812437</v>
+      </c>
+      <c r="C58" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D58" s="3">
+        <v>45509</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>14</v>
+      </c>
+      <c r="B59">
+        <v>76276156</v>
+      </c>
+      <c r="C59" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D59" s="3">
+        <v>45509</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>14</v>
+      </c>
+      <c r="B60">
+        <v>44124255</v>
+      </c>
+      <c r="C60" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D60" s="3">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>14</v>
+      </c>
+      <c r="B61">
+        <v>74319132</v>
+      </c>
+      <c r="C61" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D61" s="3">
+        <v>45527</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>14</v>
+      </c>
+      <c r="B62">
+        <v>44868164</v>
+      </c>
+      <c r="C62" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D62" s="3">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>14</v>
+      </c>
+      <c r="B63">
+        <v>74875653</v>
+      </c>
+      <c r="C63" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D63" s="3">
+        <v>45506</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>14</v>
+      </c>
+      <c r="B64">
+        <v>74379886</v>
+      </c>
+      <c r="C64" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D64" s="3">
+        <v>45511</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B65">
+        <v>70041817</v>
+      </c>
+      <c r="C65" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D65" s="3">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>14</v>
+      </c>
+      <c r="B66">
+        <v>74415593</v>
+      </c>
+      <c r="C66" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D66" s="3">
+        <v>45520</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>14</v>
+      </c>
+      <c r="B67">
+        <v>76443767</v>
+      </c>
+      <c r="C67" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D67" s="3">
+        <v>45506</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>14</v>
+      </c>
+      <c r="B68">
+        <v>75277761</v>
+      </c>
+      <c r="C68" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D68" s="3">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>14</v>
+      </c>
+      <c r="B69">
+        <v>44602153</v>
+      </c>
+      <c r="C69" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D69" s="3">
+        <v>45520</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>14</v>
+      </c>
+      <c r="B70">
+        <v>42106311</v>
+      </c>
+      <c r="C70" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D70" s="3">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>14</v>
+      </c>
+      <c r="B71">
+        <v>45477397</v>
+      </c>
+      <c r="C71" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D71" s="3">
+        <v>45518</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>14</v>
+      </c>
+      <c r="B72">
+        <v>74049235</v>
+      </c>
+      <c r="C72" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D72" s="3">
+        <v>45513</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>14</v>
+      </c>
+      <c r="B73">
+        <v>76228497</v>
+      </c>
+      <c r="C73" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D73" s="3">
+        <v>45516</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>14</v>
+      </c>
+      <c r="B74">
+        <v>73389918</v>
+      </c>
+      <c r="C74" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D74" s="3">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>14</v>
+      </c>
+      <c r="B75">
+        <v>73498771</v>
+      </c>
+      <c r="C75" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D75" s="3">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>14</v>
+      </c>
+      <c r="B76">
+        <v>71304670</v>
+      </c>
+      <c r="C76" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D76" s="3">
+        <v>45535</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>14</v>
+      </c>
+      <c r="B77">
+        <v>74457265</v>
+      </c>
+      <c r="C77" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D77" s="3">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>14</v>
+      </c>
+      <c r="B78">
+        <v>70536897</v>
+      </c>
+      <c r="C78" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D78" s="3">
+        <v>45520</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>14</v>
+      </c>
+      <c r="B79">
+        <v>77479650</v>
+      </c>
+      <c r="C79" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D79" s="3">
+        <v>45516</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>14</v>
+      </c>
+      <c r="B80">
+        <v>74968815</v>
+      </c>
+      <c r="C80" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D80" s="3">
+        <v>45506</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>14</v>
+      </c>
+      <c r="B81">
+        <v>47100567</v>
+      </c>
+      <c r="C81" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D81" s="3">
+        <v>45514</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>14</v>
+      </c>
+      <c r="B82">
+        <v>47555717</v>
+      </c>
+      <c r="C82" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D82" s="3">
+        <v>45514</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>14</v>
+      </c>
+      <c r="B83">
+        <v>48048143</v>
+      </c>
+      <c r="C83" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D83" s="3">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>14</v>
+      </c>
+      <c r="B84">
+        <v>48297098</v>
+      </c>
+      <c r="C84" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D84" s="3">
+        <v>45512</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>14</v>
+      </c>
+      <c r="B85">
+        <v>42573520</v>
+      </c>
+      <c r="C85" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D85" s="3">
+        <v>45506</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>14</v>
+      </c>
+      <c r="B86">
+        <v>75248592</v>
+      </c>
+      <c r="C86" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D86" s="3">
+        <v>45523</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>14</v>
+      </c>
+      <c r="B87">
+        <v>70989329</v>
+      </c>
+      <c r="C87" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D87" s="3">
+        <v>45535</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>14</v>
+      </c>
+      <c r="B88">
+        <v>75813343</v>
+      </c>
+      <c r="C88" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D88" s="3">
+        <v>45514</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>14</v>
+      </c>
+      <c r="B89">
+        <v>76208742</v>
+      </c>
+      <c r="C89" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D89" s="3">
+        <v>45514</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>14</v>
+      </c>
+      <c r="B90">
+        <v>72193079</v>
+      </c>
+      <c r="C90" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D90" s="3">
+        <v>45509</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>14</v>
+      </c>
+      <c r="B91">
+        <v>72839447</v>
+      </c>
+      <c r="C91" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D91" s="3">
+        <v>45523</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>14</v>
+      </c>
+      <c r="B92">
+        <v>77270950</v>
+      </c>
+      <c r="C92" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D92" s="3">
+        <v>45523</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>14</v>
+      </c>
+      <c r="B93">
+        <v>74584625</v>
+      </c>
+      <c r="C93" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D93" s="3">
+        <v>45506</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>14</v>
+      </c>
+      <c r="B94">
+        <v>71741063</v>
+      </c>
+      <c r="C94" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D94" s="3">
+        <v>45524</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>14</v>
+      </c>
+      <c r="B95">
+        <v>75384497</v>
+      </c>
+      <c r="C95" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D95" s="3">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>14</v>
+      </c>
+      <c r="B96">
+        <v>46939939</v>
+      </c>
+      <c r="C96" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D96" s="3">
+        <v>45509</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>14</v>
+      </c>
+      <c r="B97">
+        <v>73753767</v>
+      </c>
+      <c r="C97" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D97" s="3">
+        <v>45525</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>14</v>
+      </c>
+      <c r="B98">
+        <v>45016910</v>
+      </c>
+      <c r="C98" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D98" s="3">
+        <v>45511</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>14</v>
+      </c>
+      <c r="B99">
+        <v>73231061</v>
+      </c>
+      <c r="C99" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D99" s="3">
+        <v>45515</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>14</v>
+      </c>
+      <c r="B100">
+        <v>74388508</v>
+      </c>
+      <c r="C100" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D100" s="3">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>14</v>
+      </c>
+      <c r="B101">
+        <v>78720067</v>
+      </c>
+      <c r="C101" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D101" s="3">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>14</v>
+      </c>
+      <c r="B102">
+        <v>75623556</v>
+      </c>
+      <c r="C102" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D102" s="3">
+        <v>45507</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>14</v>
+      </c>
+      <c r="B103">
+        <v>74651556</v>
+      </c>
+      <c r="C103" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D103" s="3">
+        <v>45520</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>14</v>
+      </c>
+      <c r="B104">
+        <v>73250438</v>
+      </c>
+      <c r="C104" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D104" s="3">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>14</v>
+      </c>
+      <c r="B105">
+        <v>41424787</v>
+      </c>
+      <c r="C105" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D105" s="3">
+        <v>45533</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>14</v>
+      </c>
+      <c r="B106">
+        <v>42581450</v>
+      </c>
+      <c r="C106" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D106" s="3">
+        <v>45519</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>14</v>
+      </c>
+      <c r="B107">
+        <v>45150774</v>
+      </c>
+      <c r="C107" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D107" s="3">
+        <v>45519</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>14</v>
+      </c>
+      <c r="B108">
+        <v>71335524</v>
+      </c>
+      <c r="C108" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D108" s="3">
+        <v>45511</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>14</v>
+      </c>
+      <c r="B109">
+        <v>76052394</v>
+      </c>
+      <c r="C109" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D109" s="3">
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>14</v>
+      </c>
+      <c r="B110">
+        <v>47700862</v>
+      </c>
+      <c r="C110" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D110" s="3">
+        <v>45507</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>14</v>
+      </c>
+      <c r="B111">
+        <v>72431070</v>
+      </c>
+      <c r="C111" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D111" s="3">
+        <v>45511</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>14</v>
+      </c>
+      <c r="B112">
+        <v>46087865</v>
+      </c>
+      <c r="C112" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D112" s="3">
+        <v>45506</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>14</v>
+      </c>
+      <c r="B113">
+        <v>47244115</v>
+      </c>
+      <c r="C113" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D113" s="3">
+        <v>45524</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>14</v>
+      </c>
+      <c r="B114">
+        <v>75707110</v>
+      </c>
+      <c r="C114" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D114" s="3">
+        <v>45514</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>14</v>
+      </c>
+      <c r="B115">
+        <v>75625508</v>
+      </c>
+      <c r="C115" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D115" s="3">
+        <v>45511</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>14</v>
+      </c>
+      <c r="B116">
+        <v>46892034</v>
+      </c>
+      <c r="C116" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D116" s="3">
+        <v>45506</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>14</v>
+      </c>
+      <c r="B117">
+        <v>45346101</v>
+      </c>
+      <c r="C117" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D117" s="3">
+        <v>45511</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>14</v>
+      </c>
+      <c r="B118">
+        <v>45625234</v>
+      </c>
+      <c r="C118" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D118" s="3">
+        <v>45511</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>14</v>
+      </c>
+      <c r="B119">
+        <v>74619355</v>
+      </c>
+      <c r="C119" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D119" s="3">
+        <v>45523</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>14</v>
+      </c>
+      <c r="B120">
+        <v>44188867</v>
+      </c>
+      <c r="C120" t="s">
+        <v>2935</v>
+      </c>
+      <c r="D120" s="3">
+        <v>45523</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>